<commit_message>
update AMANID work plan
An update on what has been accomplished in the AMANID work plan
</commit_message>
<xml_diff>
--- a/AmanID timeline.xlsx
+++ b/AmanID timeline.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCB6C32C-F1D1-8346-9996-C6DD38F7B832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F37B185-89CA-0A4D-9107-B19840FEB885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t xml:space="preserve"> Start Date:</t>
   </si>
@@ -95,6 +95,9 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>Create user interfaces and code interactions between user interface elements</t>
+  </si>
 </sst>
 </file>
 
@@ -104,7 +107,7 @@
     <numFmt numFmtId="164" formatCode="d"/>
     <numFmt numFmtId="165" formatCode="mmm"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -223,8 +226,15 @@
       <name val="Elephant Pro"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -315,8 +325,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -532,17 +547,6 @@
       <left style="thin">
         <color theme="2" tint="-0.249977111117893"/>
       </left>
-      <right style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -563,8 +567,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="7"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </right>
+      <top style="medium">
+        <color theme="7"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="7"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="7"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -590,8 +638,9 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -622,9 +671,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="6" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -676,13 +722,28 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="14" borderId="21" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="14" borderId="20" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="14" borderId="15" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="16" fillId="14" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -691,6 +752,33 @@
     <xf numFmtId="14" fontId="1" fillId="14" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="14" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="14" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -715,7 +803,7 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -724,55 +812,23 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="14" borderId="15" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="21" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="14" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="21" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="22" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="23" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="24" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
     <cellStyle name="Date" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Day of week" xfId="8" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Good" xfId="11" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
@@ -1474,11 +1530,11 @@
   </sheetPr>
   <dimension ref="B1:AG52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="132" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScale="132" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" style="2" customWidth="1"/>
@@ -1494,464 +1550,466 @@
     <col min="38" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:33" ht="115" customHeight="1">
+    <row r="1" spans="2:33" ht="115" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="1"/>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="56"/>
-      <c r="AE1" s="56"/>
-      <c r="AF1" s="56"/>
-      <c r="AG1" s="56"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
     </row>
-    <row r="2" spans="2:33" ht="40" customHeight="1">
-      <c r="B2" s="44"/>
-      <c r="D2" s="18" t="s">
+    <row r="2" spans="2:33" ht="40" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="37"/>
+      <c r="D2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="58">
+      <c r="E2" s="29">
         <v>45011</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="20"/>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="21"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="19"/>
+      <c r="AG2" s="20"/>
     </row>
-    <row r="3" spans="2:33" ht="25" customHeight="1">
-      <c r="B3" s="45"/>
+    <row r="3" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="38"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="2:33" ht="25" customHeight="1">
-      <c r="B4" s="45"/>
-      <c r="D4" s="31" t="s">
+    <row r="4" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B4" s="38"/>
+      <c r="D4" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57" t="s">
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57" t="s">
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="T4" s="57"/>
-      <c r="U4" s="57"/>
-      <c r="V4" s="57"/>
-      <c r="W4" s="57"/>
-      <c r="X4" s="57"/>
-      <c r="Y4" s="57"/>
-      <c r="Z4" s="57" t="s">
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="33"/>
+      <c r="W4" s="33"/>
+      <c r="X4" s="33"/>
+      <c r="Y4" s="33"/>
+      <c r="Z4" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="AA4" s="57"/>
-      <c r="AB4" s="57"/>
-      <c r="AC4" s="57"/>
-      <c r="AD4" s="57"/>
-      <c r="AE4" s="57"/>
-      <c r="AF4" s="57"/>
-      <c r="AG4" s="54" t="s">
+      <c r="AA4" s="33"/>
+      <c r="AB4" s="33"/>
+      <c r="AC4" s="33"/>
+      <c r="AD4" s="33"/>
+      <c r="AE4" s="33"/>
+      <c r="AF4" s="33"/>
+      <c r="AG4" s="30" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:33" ht="25" customHeight="1">
-      <c r="B5" s="45"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="50" t="str">
+    <row r="5" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="38"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="34" t="str">
         <f>LOWER(TEXT(E7,"mmm"))</f>
         <v>mar</v>
       </c>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50" t="str">
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34" t="str">
         <f t="shared" ref="L5" si="0">LOWER(TEXT(L7,"mmm"))</f>
         <v>apr</v>
       </c>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="50" t="str">
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34" t="str">
         <f t="shared" ref="S5" si="1">LOWER(TEXT(S7,"mmm"))</f>
         <v>apr</v>
       </c>
-      <c r="T5" s="50"/>
-      <c r="U5" s="50"/>
-      <c r="V5" s="50"/>
-      <c r="W5" s="50"/>
-      <c r="X5" s="50"/>
-      <c r="Y5" s="50"/>
-      <c r="Z5" s="50" t="str">
+      <c r="T5" s="34"/>
+      <c r="U5" s="34"/>
+      <c r="V5" s="34"/>
+      <c r="W5" s="34"/>
+      <c r="X5" s="34"/>
+      <c r="Y5" s="34"/>
+      <c r="Z5" s="34" t="str">
         <f t="shared" ref="Z5" si="2">LOWER(TEXT(Z7,"mmm"))</f>
         <v>apr</v>
       </c>
-      <c r="AA5" s="50"/>
-      <c r="AB5" s="50"/>
-      <c r="AC5" s="50"/>
-      <c r="AD5" s="50"/>
-      <c r="AE5" s="50"/>
-      <c r="AF5" s="50"/>
-      <c r="AG5" s="54"/>
+      <c r="AA5" s="34"/>
+      <c r="AB5" s="34"/>
+      <c r="AC5" s="34"/>
+      <c r="AD5" s="34"/>
+      <c r="AE5" s="34"/>
+      <c r="AF5" s="34"/>
+      <c r="AG5" s="30"/>
     </row>
-    <row r="6" spans="2:33" ht="25" customHeight="1">
-      <c r="B6" s="45"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="24" t="str">
+    <row r="6" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="38"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="23" t="str">
         <f>LOWER(TEXT(E7,"aaa"))</f>
         <v>sun</v>
       </c>
-      <c r="F6" s="24" t="str">
+      <c r="F6" s="23" t="str">
         <f t="shared" ref="F6:AF6" si="3">LOWER(TEXT(F7,"aaa"))</f>
         <v>mon</v>
       </c>
-      <c r="G6" s="24" t="str">
+      <c r="G6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>tue</v>
       </c>
-      <c r="H6" s="24" t="str">
+      <c r="H6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>wed</v>
       </c>
-      <c r="I6" s="24" t="str">
+      <c r="I6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>thu</v>
       </c>
-      <c r="J6" s="24" t="str">
+      <c r="J6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>fri</v>
       </c>
-      <c r="K6" s="24" t="str">
+      <c r="K6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>sat</v>
       </c>
-      <c r="L6" s="24" t="str">
+      <c r="L6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>sun</v>
       </c>
-      <c r="M6" s="24" t="str">
+      <c r="M6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>mon</v>
       </c>
-      <c r="N6" s="24" t="str">
+      <c r="N6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>tue</v>
       </c>
-      <c r="O6" s="24" t="str">
+      <c r="O6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>wed</v>
       </c>
-      <c r="P6" s="24" t="str">
+      <c r="P6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>thu</v>
       </c>
-      <c r="Q6" s="24" t="str">
+      <c r="Q6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>fri</v>
       </c>
-      <c r="R6" s="24" t="str">
+      <c r="R6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>sat</v>
       </c>
-      <c r="S6" s="24" t="str">
+      <c r="S6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>sun</v>
       </c>
-      <c r="T6" s="24" t="str">
+      <c r="T6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>mon</v>
       </c>
-      <c r="U6" s="24" t="str">
+      <c r="U6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>tue</v>
       </c>
-      <c r="V6" s="24" t="str">
+      <c r="V6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>wed</v>
       </c>
-      <c r="W6" s="24" t="str">
+      <c r="W6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>thu</v>
       </c>
-      <c r="X6" s="24" t="str">
+      <c r="X6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>fri</v>
       </c>
-      <c r="Y6" s="24" t="str">
+      <c r="Y6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>sat</v>
       </c>
-      <c r="Z6" s="24" t="str">
+      <c r="Z6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>sun</v>
       </c>
-      <c r="AA6" s="24" t="str">
+      <c r="AA6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>mon</v>
       </c>
-      <c r="AB6" s="24" t="str">
+      <c r="AB6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>tue</v>
       </c>
-      <c r="AC6" s="24" t="str">
+      <c r="AC6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>wed</v>
       </c>
-      <c r="AD6" s="24" t="str">
+      <c r="AD6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>thu</v>
       </c>
-      <c r="AE6" s="24" t="str">
+      <c r="AE6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>fri</v>
       </c>
-      <c r="AF6" s="24" t="str">
+      <c r="AF6" s="23" t="str">
         <f t="shared" si="3"/>
         <v>sat</v>
       </c>
-      <c r="AG6" s="54"/>
+      <c r="AG6" s="30"/>
     </row>
-    <row r="7" spans="2:33" ht="25" customHeight="1" thickBot="1">
-      <c r="B7" s="45"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="16">
+    <row r="7" spans="2:33" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="38"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="15">
         <f>E2</f>
         <v>45011</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="15">
         <f>E7+1</f>
         <v>45012</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="15">
         <f t="shared" ref="G7:R7" si="4">F7+1</f>
         <v>45013</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="15">
         <f t="shared" si="4"/>
         <v>45014</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="15">
         <f t="shared" si="4"/>
         <v>45015</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7" s="15">
         <f t="shared" si="4"/>
         <v>45016</v>
       </c>
-      <c r="K7" s="16">
+      <c r="K7" s="15">
         <f t="shared" si="4"/>
         <v>45017</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="16">
         <f t="shared" si="4"/>
         <v>45018</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="15">
         <f t="shared" si="4"/>
         <v>45019</v>
       </c>
-      <c r="N7" s="16">
+      <c r="N7" s="15">
         <f t="shared" si="4"/>
         <v>45020</v>
       </c>
-      <c r="O7" s="16">
+      <c r="O7" s="15">
         <f t="shared" si="4"/>
         <v>45021</v>
       </c>
-      <c r="P7" s="16">
+      <c r="P7" s="15">
         <f t="shared" si="4"/>
         <v>45022</v>
       </c>
-      <c r="Q7" s="16">
+      <c r="Q7" s="15">
         <f t="shared" si="4"/>
         <v>45023</v>
       </c>
-      <c r="R7" s="16">
+      <c r="R7" s="15">
         <f t="shared" si="4"/>
         <v>45024</v>
       </c>
-      <c r="S7" s="17">
+      <c r="S7" s="16">
         <f>R7+1</f>
         <v>45025</v>
       </c>
-      <c r="T7" s="16">
+      <c r="T7" s="15">
         <f t="shared" ref="T7:Z7" si="5">S7+1</f>
         <v>45026</v>
       </c>
-      <c r="U7" s="16">
+      <c r="U7" s="15">
         <f t="shared" si="5"/>
         <v>45027</v>
       </c>
-      <c r="V7" s="16">
+      <c r="V7" s="15">
         <f t="shared" si="5"/>
         <v>45028</v>
       </c>
-      <c r="W7" s="16">
+      <c r="W7" s="15">
         <f t="shared" si="5"/>
         <v>45029</v>
       </c>
-      <c r="X7" s="16">
+      <c r="X7" s="15">
         <f t="shared" si="5"/>
         <v>45030</v>
       </c>
-      <c r="Y7" s="16">
+      <c r="Y7" s="15">
         <f t="shared" si="5"/>
         <v>45031</v>
       </c>
-      <c r="Z7" s="17">
+      <c r="Z7" s="16">
         <f t="shared" si="5"/>
         <v>45032</v>
       </c>
-      <c r="AA7" s="16">
+      <c r="AA7" s="15">
         <f t="shared" ref="AA7:AE7" si="6">Z7+1</f>
         <v>45033</v>
       </c>
-      <c r="AB7" s="16">
+      <c r="AB7" s="15">
         <f t="shared" si="6"/>
         <v>45034</v>
       </c>
-      <c r="AC7" s="16">
+      <c r="AC7" s="15">
         <f t="shared" si="6"/>
         <v>45035</v>
       </c>
-      <c r="AD7" s="16">
+      <c r="AD7" s="15">
         <f t="shared" si="6"/>
         <v>45036</v>
       </c>
-      <c r="AE7" s="16">
+      <c r="AE7" s="15">
         <f t="shared" si="6"/>
         <v>45037</v>
       </c>
-      <c r="AF7" s="16">
+      <c r="AF7" s="15">
         <f t="shared" ref="AF7" si="7">AE7+1</f>
         <v>45038</v>
       </c>
-      <c r="AG7" s="55"/>
+      <c r="AG7" s="31"/>
     </row>
-    <row r="8" spans="2:33" ht="25" customHeight="1">
-      <c r="B8" s="45"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="46" t="s">
+    <row r="8" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="38"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="28"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="28"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="10"/>
-      <c r="Y8" s="10"/>
-      <c r="Z8" s="10"/>
-      <c r="AA8" s="10"/>
-      <c r="AB8" s="10"/>
-      <c r="AC8" s="10"/>
-      <c r="AD8" s="10"/>
-      <c r="AE8" s="10"/>
-      <c r="AF8" s="10"/>
-      <c r="AG8" s="11" t="s">
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="60"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="60"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="60"/>
+      <c r="R8" s="60"/>
+      <c r="S8" s="60"/>
+      <c r="T8" s="60"/>
+      <c r="U8" s="60"/>
+      <c r="V8" s="57"/>
+      <c r="W8" s="57"/>
+      <c r="X8" s="57"/>
+      <c r="Y8" s="57"/>
+      <c r="Z8" s="57"/>
+      <c r="AA8" s="57"/>
+      <c r="AB8" s="57"/>
+      <c r="AC8" s="57"/>
+      <c r="AD8" s="57"/>
+      <c r="AE8" s="57"/>
+      <c r="AF8" s="58"/>
+      <c r="AG8" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:33" ht="25" customHeight="1">
-      <c r="B9" s="45"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="38" t="s">
+    <row r="9" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="38"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="23"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27"/>
+      <c r="S9" s="27"/>
+      <c r="T9" s="22"/>
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
@@ -1964,30 +2022,30 @@
       <c r="AD9" s="6"/>
       <c r="AE9" s="6"/>
       <c r="AF9" s="6"/>
-      <c r="AG9" s="12" t="s">
+      <c r="AG9" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:33" ht="25" customHeight="1">
-      <c r="B10" s="45"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="23"/>
+    <row r="10" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="38"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="22"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
-      <c r="K10" s="41" t="s">
+      <c r="K10" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="42"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="42"/>
-      <c r="R10" s="42"/>
-      <c r="S10" s="43"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="55"/>
+      <c r="O10" s="55"/>
+      <c r="P10" s="55"/>
+      <c r="Q10" s="55"/>
+      <c r="R10" s="55"/>
+      <c r="S10" s="56"/>
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
@@ -2001,14 +2059,14 @@
       <c r="AD10" s="6"/>
       <c r="AE10" s="6"/>
       <c r="AF10" s="6"/>
-      <c r="AG10" s="12" t="s">
+      <c r="AG10" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:33" ht="25" customHeight="1">
-      <c r="B11" s="45"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="23"/>
+    <row r="11" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="38"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="22"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -2018,17 +2076,17 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="48"/>
-      <c r="Q11" s="48"/>
-      <c r="R11" s="48"/>
-      <c r="S11" s="48"/>
-      <c r="T11" s="48"/>
-      <c r="U11" s="48"/>
-      <c r="V11" s="48"/>
-      <c r="W11" s="48"/>
-      <c r="X11" s="48"/>
-      <c r="Y11" s="48"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="41"/>
+      <c r="S11" s="41"/>
+      <c r="T11" s="41"/>
+      <c r="U11" s="41"/>
+      <c r="V11" s="41"/>
+      <c r="W11" s="41"/>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="41"/>
       <c r="Z11" s="6"/>
       <c r="AA11" s="6"/>
       <c r="AB11" s="6"/>
@@ -2036,371 +2094,371 @@
       <c r="AD11" s="6"/>
       <c r="AE11" s="6"/>
       <c r="AF11" s="6"/>
-      <c r="AG11" s="13" t="s">
+      <c r="AG11" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:33" ht="25" customHeight="1">
-      <c r="B12" s="45"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="40"/>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="40"/>
-      <c r="R12" s="40"/>
-      <c r="S12" s="40"/>
-      <c r="T12" s="40"/>
-      <c r="U12" s="27"/>
-      <c r="V12" s="27"/>
-      <c r="W12" s="27"/>
-      <c r="X12" s="27"/>
-      <c r="Y12" s="49"/>
-      <c r="Z12" s="49"/>
-      <c r="AA12" s="49"/>
-      <c r="AB12" s="49"/>
-      <c r="AC12" s="49"/>
-      <c r="AD12" s="49"/>
-      <c r="AE12" s="27"/>
-      <c r="AF12" s="27"/>
-      <c r="AG12" s="14" t="s">
+    <row r="12" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="38"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="53"/>
+      <c r="P12" s="53"/>
+      <c r="Q12" s="53"/>
+      <c r="R12" s="53"/>
+      <c r="S12" s="53"/>
+      <c r="T12" s="53"/>
+      <c r="U12" s="26"/>
+      <c r="V12" s="26"/>
+      <c r="W12" s="26"/>
+      <c r="X12" s="26"/>
+      <c r="Y12" s="42"/>
+      <c r="Z12" s="42"/>
+      <c r="AA12" s="42"/>
+      <c r="AB12" s="42"/>
+      <c r="AC12" s="42"/>
+      <c r="AD12" s="42"/>
+      <c r="AE12" s="26"/>
+      <c r="AF12" s="26"/>
+      <c r="AG12" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:33" ht="25" customHeight="1">
-      <c r="B13" s="45"/>
-      <c r="D13" s="31" t="s">
+    <row r="13" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="38"/>
+      <c r="D13" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="51" t="s">
+      <c r="E13" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="52" t="s">
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="M13" s="52"/>
-      <c r="N13" s="52"/>
-      <c r="O13" s="52"/>
-      <c r="P13" s="52"/>
-      <c r="Q13" s="52"/>
-      <c r="R13" s="52"/>
-      <c r="S13" s="52" t="s">
+      <c r="M13" s="44"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="44"/>
+      <c r="Q13" s="44"/>
+      <c r="R13" s="44"/>
+      <c r="S13" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="T13" s="52"/>
-      <c r="U13" s="52"/>
-      <c r="V13" s="52"/>
-      <c r="W13" s="52"/>
-      <c r="X13" s="52"/>
-      <c r="Y13" s="52"/>
-      <c r="Z13" s="52" t="s">
+      <c r="T13" s="44"/>
+      <c r="U13" s="44"/>
+      <c r="V13" s="44"/>
+      <c r="W13" s="44"/>
+      <c r="X13" s="44"/>
+      <c r="Y13" s="44"/>
+      <c r="Z13" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="AA13" s="52"/>
-      <c r="AB13" s="52"/>
-      <c r="AC13" s="52"/>
-      <c r="AD13" s="52"/>
-      <c r="AE13" s="52"/>
-      <c r="AF13" s="52"/>
-      <c r="AG13" s="25"/>
+      <c r="AA13" s="44"/>
+      <c r="AB13" s="44"/>
+      <c r="AC13" s="44"/>
+      <c r="AD13" s="44"/>
+      <c r="AE13" s="44"/>
+      <c r="AF13" s="44"/>
+      <c r="AG13" s="24"/>
     </row>
-    <row r="14" spans="2:33" ht="25" customHeight="1">
-      <c r="B14" s="45"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="53" t="str">
+    <row r="14" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="38"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="45" t="str">
         <f>LOWER(TEXT(E16,"mmm"))</f>
         <v>jan</v>
       </c>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="50" t="str">
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34" t="str">
         <f t="shared" ref="L14" si="8">LOWER(TEXT(L16,"mmm"))</f>
         <v>jan</v>
       </c>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50"/>
-      <c r="O14" s="50"/>
-      <c r="P14" s="50"/>
-      <c r="Q14" s="50"/>
-      <c r="R14" s="50"/>
-      <c r="S14" s="50" t="str">
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="34" t="str">
         <f t="shared" ref="S14" si="9">LOWER(TEXT(S16,"mmm"))</f>
         <v>jan</v>
       </c>
-      <c r="T14" s="50"/>
-      <c r="U14" s="50"/>
-      <c r="V14" s="50"/>
-      <c r="W14" s="50"/>
-      <c r="X14" s="50"/>
-      <c r="Y14" s="50"/>
-      <c r="Z14" s="50" t="str">
+      <c r="T14" s="34"/>
+      <c r="U14" s="34"/>
+      <c r="V14" s="34"/>
+      <c r="W14" s="34"/>
+      <c r="X14" s="34"/>
+      <c r="Y14" s="34"/>
+      <c r="Z14" s="34" t="str">
         <f t="shared" ref="Z14" si="10">LOWER(TEXT(Z16,"mmm"))</f>
         <v>jan</v>
       </c>
-      <c r="AA14" s="50"/>
-      <c r="AB14" s="50"/>
-      <c r="AC14" s="50"/>
-      <c r="AD14" s="50"/>
-      <c r="AE14" s="50"/>
-      <c r="AF14" s="50"/>
-      <c r="AG14" s="25"/>
+      <c r="AA14" s="34"/>
+      <c r="AB14" s="34"/>
+      <c r="AC14" s="34"/>
+      <c r="AD14" s="34"/>
+      <c r="AE14" s="34"/>
+      <c r="AF14" s="34"/>
+      <c r="AG14" s="24"/>
     </row>
-    <row r="15" spans="2:33" ht="25" customHeight="1">
-      <c r="B15" s="45"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="30" t="str">
+    <row r="15" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="38"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="28" t="str">
         <f>LOWER(TEXT(E16,"aaa"))</f>
         <v>sat</v>
       </c>
-      <c r="F15" s="24" t="str">
+      <c r="F15" s="23" t="str">
         <f t="shared" ref="F15:AF15" si="11">LOWER(TEXT(F16,"aaa"))</f>
         <v>sun</v>
       </c>
-      <c r="G15" s="24" t="str">
+      <c r="G15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>mon</v>
       </c>
-      <c r="H15" s="24" t="str">
+      <c r="H15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>tue</v>
       </c>
-      <c r="I15" s="24" t="str">
+      <c r="I15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>wed</v>
       </c>
-      <c r="J15" s="24" t="str">
+      <c r="J15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>thu</v>
       </c>
-      <c r="K15" s="24" t="str">
+      <c r="K15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>fri</v>
       </c>
-      <c r="L15" s="24" t="str">
+      <c r="L15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>sat</v>
       </c>
-      <c r="M15" s="24" t="str">
+      <c r="M15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>sun</v>
       </c>
-      <c r="N15" s="24" t="str">
+      <c r="N15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>mon</v>
       </c>
-      <c r="O15" s="24" t="str">
+      <c r="O15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>tue</v>
       </c>
-      <c r="P15" s="24" t="str">
+      <c r="P15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>wed</v>
       </c>
-      <c r="Q15" s="24" t="str">
+      <c r="Q15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>thu</v>
       </c>
-      <c r="R15" s="24" t="str">
+      <c r="R15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>fri</v>
       </c>
-      <c r="S15" s="24" t="str">
+      <c r="S15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>sat</v>
       </c>
-      <c r="T15" s="24" t="str">
+      <c r="T15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>sun</v>
       </c>
-      <c r="U15" s="24" t="str">
+      <c r="U15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>mon</v>
       </c>
-      <c r="V15" s="24" t="str">
+      <c r="V15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>tue</v>
       </c>
-      <c r="W15" s="24" t="str">
+      <c r="W15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>wed</v>
       </c>
-      <c r="X15" s="24" t="str">
+      <c r="X15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>thu</v>
       </c>
-      <c r="Y15" s="24" t="str">
+      <c r="Y15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>fri</v>
       </c>
-      <c r="Z15" s="24" t="str">
+      <c r="Z15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>sat</v>
       </c>
-      <c r="AA15" s="24" t="str">
+      <c r="AA15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>sun</v>
       </c>
-      <c r="AB15" s="24" t="str">
+      <c r="AB15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>mon</v>
       </c>
-      <c r="AC15" s="24" t="str">
+      <c r="AC15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>tue</v>
       </c>
-      <c r="AD15" s="24" t="str">
+      <c r="AD15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>wed</v>
       </c>
-      <c r="AE15" s="24" t="str">
+      <c r="AE15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>thu</v>
       </c>
-      <c r="AF15" s="24" t="str">
+      <c r="AF15" s="23" t="str">
         <f t="shared" si="11"/>
         <v>fri</v>
       </c>
-      <c r="AG15" s="25"/>
+      <c r="AG15" s="24"/>
     </row>
-    <row r="16" spans="2:33" ht="25" customHeight="1" thickBot="1">
-      <c r="B16" s="45"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="16">
+    <row r="16" spans="2:33" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="38"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="15">
         <f>E11</f>
         <v>0</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="15">
         <f>E16+1</f>
         <v>1</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G16" s="15">
         <f t="shared" ref="G16" si="12">F16+1</f>
         <v>2</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="15">
         <f t="shared" ref="H16" si="13">G16+1</f>
         <v>3</v>
       </c>
-      <c r="I16" s="16">
+      <c r="I16" s="15">
         <f t="shared" ref="I16" si="14">H16+1</f>
         <v>4</v>
       </c>
-      <c r="J16" s="16">
+      <c r="J16" s="15">
         <f t="shared" ref="J16" si="15">I16+1</f>
         <v>5</v>
       </c>
-      <c r="K16" s="16">
+      <c r="K16" s="15">
         <f t="shared" ref="K16" si="16">J16+1</f>
         <v>6</v>
       </c>
-      <c r="L16" s="17">
+      <c r="L16" s="16">
         <f t="shared" ref="L16" si="17">K16+1</f>
         <v>7</v>
       </c>
-      <c r="M16" s="16">
+      <c r="M16" s="15">
         <f t="shared" ref="M16" si="18">L16+1</f>
         <v>8</v>
       </c>
-      <c r="N16" s="16">
+      <c r="N16" s="15">
         <f t="shared" ref="N16" si="19">M16+1</f>
         <v>9</v>
       </c>
-      <c r="O16" s="16">
+      <c r="O16" s="15">
         <f t="shared" ref="O16" si="20">N16+1</f>
         <v>10</v>
       </c>
-      <c r="P16" s="16">
+      <c r="P16" s="15">
         <f t="shared" ref="P16" si="21">O16+1</f>
         <v>11</v>
       </c>
-      <c r="Q16" s="16">
+      <c r="Q16" s="15">
         <f t="shared" ref="Q16" si="22">P16+1</f>
         <v>12</v>
       </c>
-      <c r="R16" s="16">
+      <c r="R16" s="15">
         <f t="shared" ref="R16" si="23">Q16+1</f>
         <v>13</v>
       </c>
-      <c r="S16" s="17">
+      <c r="S16" s="16">
         <f>R16+1</f>
         <v>14</v>
       </c>
-      <c r="T16" s="16">
+      <c r="T16" s="15">
         <f t="shared" ref="T16" si="24">S16+1</f>
         <v>15</v>
       </c>
-      <c r="U16" s="16">
+      <c r="U16" s="15">
         <f t="shared" ref="U16" si="25">T16+1</f>
         <v>16</v>
       </c>
-      <c r="V16" s="16">
+      <c r="V16" s="15">
         <f t="shared" ref="V16" si="26">U16+1</f>
         <v>17</v>
       </c>
-      <c r="W16" s="16">
+      <c r="W16" s="15">
         <f t="shared" ref="W16" si="27">V16+1</f>
         <v>18</v>
       </c>
-      <c r="X16" s="16">
+      <c r="X16" s="15">
         <f t="shared" ref="X16" si="28">W16+1</f>
         <v>19</v>
       </c>
-      <c r="Y16" s="16">
+      <c r="Y16" s="15">
         <f t="shared" ref="Y16" si="29">X16+1</f>
         <v>20</v>
       </c>
-      <c r="Z16" s="17">
+      <c r="Z16" s="16">
         <f t="shared" ref="Z16" si="30">Y16+1</f>
         <v>21</v>
       </c>
-      <c r="AA16" s="16">
+      <c r="AA16" s="15">
         <f t="shared" ref="AA16" si="31">Z16+1</f>
         <v>22</v>
       </c>
-      <c r="AB16" s="16">
+      <c r="AB16" s="15">
         <f t="shared" ref="AB16" si="32">AA16+1</f>
         <v>23</v>
       </c>
-      <c r="AC16" s="16">
+      <c r="AC16" s="15">
         <f t="shared" ref="AC16" si="33">AB16+1</f>
         <v>24</v>
       </c>
-      <c r="AD16" s="16">
+      <c r="AD16" s="15">
         <f t="shared" ref="AD16" si="34">AC16+1</f>
         <v>25</v>
       </c>
-      <c r="AE16" s="16">
+      <c r="AE16" s="15">
         <f t="shared" ref="AE16" si="35">AD16+1</f>
         <v>26</v>
       </c>
-      <c r="AF16" s="16">
+      <c r="AF16" s="15">
         <f t="shared" ref="AF16" si="36">AE16+1</f>
         <v>27</v>
       </c>
       <c r="AG16" s="7"/>
     </row>
-    <row r="17" spans="2:33" ht="25" customHeight="1">
-      <c r="B17" s="45"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="23"/>
+    <row r="17" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="38"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="22"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -2430,10 +2488,10 @@
       <c r="AF17" s="6"/>
       <c r="AG17" s="7"/>
     </row>
-    <row r="18" spans="2:33" ht="25" customHeight="1">
-      <c r="B18" s="45"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="23"/>
+    <row r="18" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="38"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="22"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -2463,10 +2521,10 @@
       <c r="AF18" s="6"/>
       <c r="AG18" s="7"/>
     </row>
-    <row r="19" spans="2:33" ht="25" customHeight="1">
-      <c r="B19" s="45"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="23"/>
+    <row r="19" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="38"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="22"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -2496,10 +2554,10 @@
       <c r="AF19" s="6"/>
       <c r="AG19" s="7"/>
     </row>
-    <row r="20" spans="2:33" ht="25" customHeight="1">
-      <c r="B20" s="45"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="23"/>
+    <row r="20" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="38"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="22"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -2529,20 +2587,20 @@
       <c r="AF20" s="6"/>
       <c r="AG20" s="7"/>
     </row>
-    <row r="21" spans="2:33" ht="25" customHeight="1">
-      <c r="B21" s="45"/>
-      <c r="D21" s="22" t="s">
+    <row r="21" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="38"/>
+      <c r="D21" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
@@ -2566,19 +2624,19 @@
       <c r="AF21" s="6"/>
       <c r="AG21" s="7"/>
     </row>
-    <row r="22" spans="2:33" ht="25" customHeight="1">
-      <c r="B22" s="45"/>
+    <row r="22" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="38"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="35" t="str">
+      <c r="E22" s="48" t="str">
         <f>LOWER(TEXT(E24,"mmm"))</f>
         <v>jan</v>
       </c>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="37"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="50"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
@@ -2602,34 +2660,34 @@
       <c r="AF22" s="6"/>
       <c r="AG22" s="7"/>
     </row>
-    <row r="23" spans="2:33" ht="25" customHeight="1">
-      <c r="B23" s="45"/>
+    <row r="23" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="38"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="15" t="str">
+      <c r="E23" s="14" t="str">
         <f t="shared" ref="E23:K23" si="37">LOWER(TEXT(E24,"aaa"))</f>
         <v>sun</v>
       </c>
-      <c r="F23" s="15" t="str">
+      <c r="F23" s="14" t="str">
         <f t="shared" si="37"/>
         <v>mon</v>
       </c>
-      <c r="G23" s="15" t="str">
+      <c r="G23" s="14" t="str">
         <f t="shared" si="37"/>
         <v>tue</v>
       </c>
-      <c r="H23" s="15" t="str">
+      <c r="H23" s="14" t="str">
         <f t="shared" si="37"/>
         <v>wed</v>
       </c>
-      <c r="I23" s="15" t="str">
+      <c r="I23" s="14" t="str">
         <f t="shared" si="37"/>
         <v>thu</v>
       </c>
-      <c r="J23" s="15" t="str">
+      <c r="J23" s="14" t="str">
         <f t="shared" si="37"/>
         <v>fri</v>
       </c>
-      <c r="K23" s="15" t="str">
+      <c r="K23" s="14" t="str">
         <f t="shared" si="37"/>
         <v>sat</v>
       </c>
@@ -2656,34 +2714,34 @@
       <c r="AF23" s="6"/>
       <c r="AG23" s="7"/>
     </row>
-    <row r="24" spans="2:33" ht="25" customHeight="1" thickBot="1">
-      <c r="B24" s="45"/>
+    <row r="24" spans="2:33" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="38"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="16">
+      <c r="E24" s="15">
         <f>D25+1</f>
         <v>1</v>
       </c>
-      <c r="F24" s="16">
+      <c r="F24" s="15">
         <f t="shared" ref="F24" si="38">E24+1</f>
         <v>2</v>
       </c>
-      <c r="G24" s="16">
+      <c r="G24" s="15">
         <f t="shared" ref="G24" si="39">F24+1</f>
         <v>3</v>
       </c>
-      <c r="H24" s="16">
+      <c r="H24" s="15">
         <f t="shared" ref="H24" si="40">G24+1</f>
         <v>4</v>
       </c>
-      <c r="I24" s="16">
+      <c r="I24" s="15">
         <f t="shared" ref="I24" si="41">H24+1</f>
         <v>5</v>
       </c>
-      <c r="J24" s="16">
+      <c r="J24" s="15">
         <f t="shared" ref="J24" si="42">I24+1</f>
         <v>6</v>
       </c>
-      <c r="K24" s="16">
+      <c r="K24" s="15">
         <f t="shared" ref="K24" si="43">J24+1</f>
         <v>7</v>
       </c>
@@ -2710,8 +2768,8 @@
       <c r="AF24" s="6"/>
       <c r="AG24" s="7"/>
     </row>
-    <row r="25" spans="2:33" ht="25" customHeight="1">
-      <c r="B25" s="45"/>
+    <row r="25" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="38"/>
       <c r="D25" s="8"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
@@ -2736,8 +2794,8 @@
       <c r="AF25" s="6"/>
       <c r="AG25" s="7"/>
     </row>
-    <row r="26" spans="2:33" ht="25" customHeight="1">
-      <c r="B26" s="45"/>
+    <row r="26" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="38"/>
       <c r="D26" s="8"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
@@ -2769,8 +2827,8 @@
       <c r="AF26" s="6"/>
       <c r="AG26" s="7"/>
     </row>
-    <row r="27" spans="2:33" ht="25" customHeight="1">
-      <c r="B27" s="45"/>
+    <row r="27" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="38"/>
       <c r="D27" s="8"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
@@ -2802,8 +2860,8 @@
       <c r="AF27" s="6"/>
       <c r="AG27" s="7"/>
     </row>
-    <row r="28" spans="2:33" ht="25" customHeight="1">
-      <c r="B28" s="45"/>
+    <row r="28" spans="2:33" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="38"/>
       <c r="D28" s="8"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -2835,44 +2893,34 @@
       <c r="AF28" s="6"/>
       <c r="AG28" s="7"/>
     </row>
-    <row r="29" spans="2:33" ht="22" customHeight="1">
+    <row r="29" spans="2:33" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="2:33" ht="22" customHeight="1"/>
-    <row r="31" spans="2:33" ht="22" customHeight="1"/>
-    <row r="32" spans="2:33" ht="22" customHeight="1"/>
-    <row r="33" ht="22" customHeight="1"/>
-    <row r="34" ht="22" customHeight="1"/>
-    <row r="35" ht="22" customHeight="1"/>
-    <row r="36" ht="22" customHeight="1"/>
-    <row r="37" ht="22" customHeight="1"/>
-    <row r="38" ht="22" customHeight="1"/>
-    <row r="39" ht="22" customHeight="1"/>
-    <row r="40" ht="22" customHeight="1"/>
-    <row r="41" ht="22" customHeight="1"/>
-    <row r="42" ht="22" customHeight="1"/>
-    <row r="43" ht="22" customHeight="1"/>
-    <row r="44" ht="22" customHeight="1"/>
-    <row r="45" ht="22" customHeight="1"/>
-    <row r="46" ht="22" customHeight="1"/>
-    <row r="47" ht="22" customHeight="1"/>
-    <row r="48" ht="22" customHeight="1"/>
-    <row r="49" ht="22" customHeight="1"/>
-    <row r="50" ht="22" customHeight="1"/>
-    <row r="51" ht="22" customHeight="1"/>
-    <row r="52" ht="22" customHeight="1"/>
+    <row r="30" spans="2:33" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="31" spans="2:33" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="32" spans="2:33" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="33" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="34" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="35" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="36" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="37" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="38" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="39" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="40" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="41" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="42" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="43" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="44" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="45" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="46" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="47" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="48" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="49" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="50" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="51" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="52" ht="22" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="AG4:AG7"/>
-    <mergeCell ref="D1:AG1"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="E4:K4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="E5:K5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z5:AF5"/>
-    <mergeCell ref="D4:D12"/>
+  <mergeCells count="30">
     <mergeCell ref="B2:B28"/>
     <mergeCell ref="E8:I8"/>
     <mergeCell ref="O11:Y11"/>
@@ -2889,9 +2937,20 @@
     <mergeCell ref="D13:D20"/>
     <mergeCell ref="E21:K21"/>
     <mergeCell ref="E22:K22"/>
+    <mergeCell ref="AG4:AG7"/>
+    <mergeCell ref="D1:AG1"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="E4:K4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="E5:K5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z5:AF5"/>
+    <mergeCell ref="D4:D12"/>
     <mergeCell ref="E9:J9"/>
     <mergeCell ref="O12:T12"/>
     <mergeCell ref="K10:S10"/>
+    <mergeCell ref="J8:U8"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <conditionalFormatting sqref="E7:AF7">
@@ -3256,15 +3315,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -3282,6 +3332,15 @@
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3306,14 +3365,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BDAE179-36E2-4ABF-831B-D3EE8CCF7DCC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D72A4EE4-D1F3-4991-BFF1-8D5561410967}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3325,6 +3376,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BDAE179-36E2-4ABF-831B-D3EE8CCF7DCC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>